<commit_message>
Data populate from excel to DB
</commit_message>
<xml_diff>
--- a/server/DB_Data.xlsx
+++ b/server/DB_Data.xlsx
@@ -261,13 +261,13 @@
     <t>silambuselvan.d@gmail.com</t>
   </si>
   <si>
+    <t>Naveen</t>
+  </si>
+  <si>
+    <t>naveen@test.com</t>
+  </si>
+  <si>
     <t>user</t>
-  </si>
-  <si>
-    <t>Naveen</t>
-  </si>
-  <si>
-    <t>naveen@test.com</t>
   </si>
 </sst>
 </file>
@@ -1338,13 +1338,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="28.6363636363636" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1352,7 +1352,7 @@
     <col min="4" max="4" width="13.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.25" spans="1:4">
+    <row r="1" ht="15.25" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1362,9 +1362,8 @@
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" ht="15.25" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1374,22 +1373,6 @@
       <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1403,7 +1386,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1441,18 +1424,18 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>